<commit_message>
Se actualizan casos de prueba de app web y mobile en relacion a los cambios realizados
</commit_message>
<xml_diff>
--- a/Testing 2024/template_caso_prueba-ISPC2024-sprint-2-mobile.xlsx
+++ b/Testing 2024/template_caso_prueba-ISPC2024-sprint-2-mobile.xlsx
@@ -83,7 +83,7 @@
     <t xml:space="preserve">Visualizar bajo la barra de busqueda las categorias de los libros</t>
   </si>
   <si>
-    <t xml:space="preserve">TO DO</t>
+    <t xml:space="preserve">Reviewed</t>
   </si>
   <si>
     <t xml:space="preserve">Andrea Caligiuri</t>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t xml:space="preserve">Visualizar la barra de busqueda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TO DO</t>
   </si>
   <si>
     <t xml:space="preserve">2.</t>
@@ -162,9 +165,6 @@
   </si>
   <si>
     <t xml:space="preserve">Deberá mostrarse en pantalla un formulario de Inicio de sesion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reviewed</t>
   </si>
   <si>
     <t xml:space="preserve">TC-006</t>
@@ -1142,22 +1142,22 @@
   <dimension ref="A1:AA846"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H26" activeCellId="0" sqref="H26"/>
+      <selection pane="topLeft" activeCell="K72" activeCellId="0" sqref="K72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="24.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="5.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="51.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="12" style="0" width="15.71"/>
   </cols>
   <sheetData>
@@ -1572,7 +1572,7 @@
       </c>
       <c r="H12" s="14"/>
       <c r="I12" s="16" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="J12" s="14" t="s">
         <v>21</v>
@@ -1604,13 +1604,13 @@
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
       <c r="F13" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I13" s="16"/>
       <c r="J13" s="14"/>
@@ -1692,16 +1692,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B16" s="14" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E16" s="14" t="s">
         <v>31</v>
@@ -1714,7 +1714,7 @@
       </c>
       <c r="H16" s="14"/>
       <c r="I16" s="16" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="J16" s="14" t="s">
         <v>21</v>
@@ -1746,13 +1746,13 @@
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
       <c r="F17" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I17" s="16"/>
       <c r="J17" s="14"/>
@@ -1834,31 +1834,31 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F20" s="15" t="s">
         <v>17</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I20" s="16" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="J20" s="14" t="s">
         <v>21</v>
@@ -1975,7 +1975,7 @@
         <v>48</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C24" s="14" t="s">
         <v>49</v>
@@ -1984,7 +1984,7 @@
         <v>50</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F24" s="15" t="s">
         <v>17</v>
@@ -1996,7 +1996,7 @@
         <v>52</v>
       </c>
       <c r="I24" s="16" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="J24" s="14" t="s">
         <v>21</v>
@@ -2113,7 +2113,7 @@
         <v>53</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C28" s="14" t="s">
         <v>54</v>
@@ -2134,7 +2134,7 @@
         <v>58</v>
       </c>
       <c r="I28" s="16" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="J28" s="14" t="s">
         <v>21</v>
@@ -2166,7 +2166,7 @@
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
       <c r="F29" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G29" s="14" t="s">
         <v>59</v>
@@ -2263,7 +2263,7 @@
         <v>64</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C32" s="14" t="s">
         <v>65</v>
@@ -2278,13 +2278,13 @@
         <v>17</v>
       </c>
       <c r="G32" s="14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H32" s="14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I32" s="16" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="J32" s="14" t="s">
         <v>21</v>
@@ -2316,7 +2316,7 @@
       <c r="D33" s="14"/>
       <c r="E33" s="14"/>
       <c r="F33" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G33" s="14" t="s">
         <v>68</v>
@@ -2413,7 +2413,7 @@
         <v>71</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C36" s="14" t="s">
         <v>72</v>
@@ -2431,10 +2431,10 @@
         <v>75</v>
       </c>
       <c r="H36" s="14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I36" s="16" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="J36" s="14" t="s">
         <v>76</v>
@@ -2466,7 +2466,7 @@
       <c r="D37" s="14"/>
       <c r="E37" s="14"/>
       <c r="F37" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G37" s="14" t="s">
         <v>77</v>
@@ -2563,7 +2563,7 @@
         <v>80</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C40" s="14" t="s">
         <v>81</v>
@@ -2581,10 +2581,10 @@
         <v>75</v>
       </c>
       <c r="H40" s="14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I40" s="16" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="J40" s="14" t="s">
         <v>76</v>
@@ -2616,7 +2616,7 @@
       <c r="D41" s="14"/>
       <c r="E41" s="14"/>
       <c r="F41" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G41" s="14" t="s">
         <v>84</v>
@@ -2713,7 +2713,7 @@
         <v>85</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C44" s="14" t="s">
         <v>86</v>
@@ -2734,7 +2734,7 @@
         <v>58</v>
       </c>
       <c r="I44" s="16" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="J44" s="14" t="s">
         <v>76</v>
@@ -2766,7 +2766,7 @@
       <c r="D45" s="14"/>
       <c r="E45" s="14"/>
       <c r="F45" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G45" s="14" t="s">
         <v>89</v>
@@ -2857,7 +2857,7 @@
         <v>91</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C48" s="14" t="s">
         <v>92</v>
@@ -2878,7 +2878,7 @@
         <v>58</v>
       </c>
       <c r="I48" s="16" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="J48" s="14" t="s">
         <v>76</v>
@@ -2910,7 +2910,7 @@
       <c r="D49" s="14"/>
       <c r="E49" s="14"/>
       <c r="F49" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G49" s="14" t="s">
         <v>94</v>
@@ -3013,7 +3013,7 @@
         <v>99</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C52" s="14" t="s">
         <v>100</v>
@@ -3034,7 +3034,7 @@
         <v>58</v>
       </c>
       <c r="I52" s="16" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="J52" s="14" t="s">
         <v>76</v>
@@ -3066,7 +3066,7 @@
       <c r="D53" s="14"/>
       <c r="E53" s="14"/>
       <c r="F53" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G53" s="14" t="s">
         <v>102</v>
@@ -3190,7 +3190,7 @@
         <v>110</v>
       </c>
       <c r="I56" s="16" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="J56" s="14" t="s">
         <v>76</v>
@@ -3328,7 +3328,7 @@
         <v>115</v>
       </c>
       <c r="I60" s="16" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="J60" s="14" t="s">
         <v>76</v>
@@ -3466,7 +3466,7 @@
         <v>122</v>
       </c>
       <c r="I64" s="16" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="J64" s="14" t="s">
         <v>76</v>
@@ -3556,7 +3556,7 @@
       <c r="D67" s="14"/>
       <c r="E67" s="14"/>
       <c r="F67" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G67" s="25"/>
       <c r="H67" s="25"/>
@@ -3606,7 +3606,7 @@
         <v>128</v>
       </c>
       <c r="I68" s="16" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="J68" s="14" t="s">
         <v>76</v>
@@ -3696,7 +3696,7 @@
       <c r="D71" s="14"/>
       <c r="E71" s="14"/>
       <c r="F71" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G71" s="15"/>
       <c r="H71" s="15"/>
@@ -3746,7 +3746,7 @@
         <v>134</v>
       </c>
       <c r="I72" s="16" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="J72" s="14" t="s">
         <v>76</v>
@@ -3836,7 +3836,7 @@
       <c r="D75" s="14"/>
       <c r="E75" s="14"/>
       <c r="F75" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G75" s="15"/>
       <c r="H75" s="15"/>
@@ -3886,7 +3886,7 @@
         <v>140</v>
       </c>
       <c r="I76" s="16" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="J76" s="14" t="s">
         <v>76</v>
@@ -3947,7 +3947,7 @@
       <c r="D78" s="14"/>
       <c r="E78" s="14"/>
       <c r="F78" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G78" s="15"/>
       <c r="H78" s="15"/>
@@ -26534,7 +26534,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="1" style="0" width="15.71"/>
   </cols>

</xml_diff>